<commit_message>
march 17 1047am update
</commit_message>
<xml_diff>
--- a/Jupyter/simulationID/cim_0315_1240/data/bldg/polygon_502_0147678.xlsx
+++ b/Jupyter/simulationID/cim_0315_1240/data/bldg/polygon_502_0147678.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shai/Google Drive/BatYam NY DRIVE/Simulations/March 14 GitHUB/BatYamNY/Jupyter/simulationID/cim_0315_1240/data/bldg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C39683C-7CDA-EC41-91F5-C8AF1A39C352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510BCB5B-4BEB-984A-A8C8-225374781C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33740" yWindow="-2680" windowWidth="23800" windowHeight="20540" xr2:uid="{09545E3B-D688-BC4E-A3A4-20D3E9254CDF}"/>
   </bookViews>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A862755-D32A-7647-802C-521691023E49}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>